<commit_message>
Changes in the tone control
</commit_message>
<xml_diff>
--- a/products/measurement_reports/tone_control/measurement/measurement_tone_control.xlsx
+++ b/products/measurement_reports/tone_control/measurement/measurement_tone_control.xlsx
@@ -403,11 +403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131710080"/>
-        <c:axId val="131709520"/>
+        <c:axId val="118314400"/>
+        <c:axId val="118314960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131710080"/>
+        <c:axId val="118314400"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -521,12 +521,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131709520"/>
+        <c:crossAx val="118314960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131709520"/>
+        <c:axId val="118314960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -646,7 +646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131710080"/>
+        <c:crossAx val="118314400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -998,11 +998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131715120"/>
-        <c:axId val="131715680"/>
+        <c:axId val="156474288"/>
+        <c:axId val="156474848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131715120"/>
+        <c:axId val="156474288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1121,12 +1121,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131715680"/>
+        <c:crossAx val="156474848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131715680"/>
+        <c:axId val="156474848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1239,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131715120"/>
+        <c:crossAx val="156474288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1409,10 +1409,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$28</c:f>
+              <c:f>Sheet1!$C$5:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1423,66 +1423,75 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>2500</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>7500</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>9000</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>25000</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>200000</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>300000</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>400000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1490,81 +1499,90 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$28</c:f>
+              <c:f>Sheet1!$G$5:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-3.3266284353304991</c:v>
+                  <c:v>-3.6728879389225417</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.910253356282996</c:v>
+                  <c:v>-4.9864634518020958</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.5193746454456232</c:v>
+                  <c:v>-7.7636034276576282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.2648286954916266</c:v>
+                  <c:v>-7.8086081378658401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.4726132101604894</c:v>
+                  <c:v>-6.3253992444143599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.3681573889868428</c:v>
+                  <c:v>-5.4476962842890222</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>-3.6728879389225417</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.5321179195152581</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.83784322656354093</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.74648646047624689</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.50221441166062175</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.20200653808651459</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>-0.71995306543037696</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.1996844181320179</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.3994216186124</c:v>
+                  <c:v>-0.6133763953290382</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.5050190483838484</c:v>
+                  <c:v>-1.8644864686218674</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.5633541347699684</c:v>
+                  <c:v>-2.2394751888786453</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.6939714779491233</c:v>
+                  <c:v>-3.2812034326829149</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.6939714779491233</c:v>
+                  <c:v>-5.3629753853865116</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.5306495922971446</c:v>
+                  <c:v>-7.0436503622272495</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2.7899491355844974</c:v>
+                  <c:v>-7.8167933650819723</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.129106618285737</c:v>
+                  <c:v>-7.8167933650819723</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.5857875220397516</c:v>
+                  <c:v>-8.3582217920531523</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.1190281065829994</c:v>
+                  <c:v>-8.0547778310761267</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-1.4171171452698736</c:v>
+                  <c:v>-6.3117743166981235</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-5.3769062458515968</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-5.8337993881967556</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-6.8107707389530958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1579,11 +1597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131717920"/>
-        <c:axId val="131718480"/>
+        <c:axId val="156477088"/>
+        <c:axId val="156477648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131717920"/>
+        <c:axId val="156477088"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1702,12 +1720,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131718480"/>
+        <c:crossAx val="156477648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131718480"/>
+        <c:axId val="156477648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1838,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131717920"/>
+        <c:crossAx val="156477088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3542,15 +3560,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>6723</xdr:rowOff>
+      <xdr:colOff>60104</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>127950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>705970</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>82923</xdr:rowOff>
+      <xdr:colOff>654015</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>13650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3602,15 +3620,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>112058</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>163606</xdr:rowOff>
+      <xdr:colOff>8148</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>163605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>313764</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>49306</xdr:rowOff>
+      <xdr:colOff>209854</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>49305</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3921,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,18 +4028,18 @@
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>0.06</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5/D5</f>
-        <v>0.68181818181818188</v>
+        <v>0.65517241379310354</v>
       </c>
       <c r="G5" s="1">
         <f>20*LOG10(F5)</f>
-        <v>-3.3266284353304991</v>
+        <v>-3.6728879389225417</v>
       </c>
       <c r="I5" s="1">
         <v>2</v>
@@ -4063,18 +4081,18 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>0.05</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6/D6</f>
-        <v>0.56818181818181823</v>
+        <v>0.56321839080459779</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" ref="G6:G30" si="0">20*LOG10(F6)</f>
-        <v>-4.910253356282996</v>
+        <f t="shared" ref="G6:G31" si="0">20*LOG10(F6)</f>
+        <v>-4.9864634518020958</v>
       </c>
       <c r="I6" s="1">
         <v>10</v>
@@ -4116,18 +4134,18 @@
         <v>25</v>
       </c>
       <c r="D7" s="1">
-        <v>0.08</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>0.03</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ref="F7:F18" si="3">E7/D7</f>
-        <v>0.375</v>
+        <v>0.40909090909090906</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>-8.5193746454456232</v>
+        <v>-7.7636034276576282</v>
       </c>
       <c r="I7" s="1">
         <v>25</v>
@@ -4166,21 +4184,21 @@
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
-        <v>0.54545454545454553</v>
+        <v>0.40697674418604657</v>
       </c>
       <c r="G8" s="1">
         <f>20*LOG10(F8)</f>
-        <v>-5.2648286954916266</v>
+        <v>-7.8086081378658401</v>
       </c>
       <c r="I8" s="1">
         <v>50</v>
@@ -4219,21 +4237,21 @@
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>5.8999999999999997E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="3"/>
-        <v>0.67045454545454541</v>
+        <v>0.48275862068965525</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>-3.4726132101604894</v>
+        <v>-6.3253992444143599</v>
       </c>
       <c r="I9" s="1">
         <v>75</v>
@@ -4272,21 +4290,21 @@
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="3"/>
-        <v>0.76136363636363646</v>
+        <v>0.53409090909090917</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>-2.3681573889868428</v>
+        <v>-5.4476962842890222</v>
       </c>
       <c r="I10" s="1">
         <v>100</v>
@@ -4325,21 +4343,21 @@
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>8.1000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="3"/>
-        <v>0.92045454545454553</v>
+        <v>0.65517241379310354</v>
       </c>
       <c r="G11" s="1">
         <f>20*LOG10(F11)</f>
-        <v>-0.71995306543037696</v>
+        <v>-3.6728879389225417</v>
       </c>
       <c r="I11" s="1">
         <v>200</v>
@@ -4378,21 +4396,21 @@
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="3"/>
-        <v>0.97727272727272729</v>
+        <v>0.74712643678160928</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.1996844181320179</v>
+        <v>-2.5321179195152581</v>
       </c>
       <c r="I12" s="1">
         <v>300</v>
@@ -4431,21 +4449,21 @@
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.90804597701149437</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.83784322656354093</v>
       </c>
       <c r="I13" s="1">
         <v>400</v>
@@ -4484,21 +4502,21 @@
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D14" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.91764705882352937</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.74648646047624689</v>
       </c>
       <c r="I14" s="1">
         <v>500</v>
@@ -4537,21 +4555,21 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="D15" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.94382022471910121</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.50221441166062175</v>
       </c>
       <c r="I15" s="1">
         <v>750</v>
@@ -4590,21 +4608,21 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D16" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.9770114942528737</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.20200653808651459</v>
       </c>
       <c r="I16" s="1">
         <v>1000</v>
@@ -4643,21 +4661,21 @@
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
-        <v>2000</v>
+        <v>750</v>
       </c>
       <c r="D17" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E17" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.92045454545454553</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.71995306543037696</v>
       </c>
       <c r="I17" s="1">
         <v>2000</v>
@@ -4696,21 +4714,21 @@
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="D18" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>8.5000000000000006E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="3"/>
-        <v>0.95505617977528101</v>
+        <v>0.93181818181818188</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.3994216186124</v>
+        <v>-0.6133763953290382</v>
       </c>
       <c r="I18" s="1">
         <v>2500</v>
@@ -4749,21 +4767,21 @@
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="D19" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ref="F19:F28" si="6">E19/D19</f>
-        <v>0.84090909090909094</v>
+        <v>0.80681818181818177</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ref="G19:G28" si="7">20*LOG10(F19)</f>
-        <v>-1.5050190483838484</v>
+        <v>-1.8644864686218674</v>
       </c>
       <c r="I19" s="1">
         <v>3000</v>
@@ -4802,21 +4820,21 @@
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <v>7500</v>
+        <v>2500</v>
       </c>
       <c r="D20" s="1">
-        <v>0.09</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="6"/>
-        <v>0.74444444444444446</v>
+        <v>0.77272727272727282</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="7"/>
-        <v>-2.5633541347699684</v>
+        <v>-2.2394751888786453</v>
       </c>
       <c r="I20" s="1">
         <v>5000</v>
@@ -4855,21 +4873,21 @@
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="D21" s="1">
-        <v>0.09</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E21" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="6"/>
-        <v>0.73333333333333339</v>
+        <v>0.6853932584269663</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="7"/>
-        <v>-2.6939714779491233</v>
+        <v>-3.2812034326829149</v>
       </c>
       <c r="I21" s="1">
         <v>7500</v>
@@ -4908,21 +4926,21 @@
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D22" s="1">
-        <v>0.09</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E22" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="6"/>
-        <v>0.73333333333333339</v>
+        <v>0.5393258426966292</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="7"/>
-        <v>-2.6939714779491233</v>
+        <v>-5.3629753853865116</v>
       </c>
       <c r="I22" s="1">
         <v>9000</v>
@@ -4961,21 +4979,21 @@
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>25000</v>
+        <v>7500</v>
       </c>
       <c r="D23" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E23" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="6"/>
-        <v>0.74725274725274737</v>
+        <v>0.44444444444444448</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="7"/>
-        <v>-2.5306495922971446</v>
+        <v>-7.0436503622272495</v>
       </c>
       <c r="I23" s="1">
         <v>10000</v>
@@ -5014,21 +5032,21 @@
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
-        <v>50000</v>
+        <v>9000</v>
       </c>
       <c r="D24" s="1">
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="6"/>
-        <v>0.72527472527472536</v>
+        <v>0.40659340659340659</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="7"/>
-        <v>-2.7899491355844974</v>
+        <v>-7.8167933650819723</v>
       </c>
       <c r="I24" s="1">
         <v>25000</v>
@@ -5067,21 +5085,21 @@
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="D25" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>7.1999999999999995E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="6"/>
-        <v>0.78260869565217384</v>
+        <v>0.40659340659340659</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="7"/>
-        <v>-2.129106618285737</v>
+        <v>-7.8167933650819723</v>
       </c>
       <c r="I25" s="1">
         <v>50000</v>
@@ -5120,21 +5138,21 @@
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
-        <v>200000</v>
+        <v>25000</v>
       </c>
       <c r="D26" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E26" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="6"/>
-        <v>0.93478260869565211</v>
+        <v>0.3820224719101124</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="7"/>
-        <v>-0.5857875220397516</v>
+        <v>-8.3582217920531523</v>
       </c>
       <c r="I26" s="1">
         <v>100000</v>
@@ -5173,21 +5191,21 @@
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>300000</v>
+        <v>50000</v>
       </c>
       <c r="D27" s="1">
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E27" s="1">
-        <v>0.08</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="6"/>
-        <v>0.87912087912087922</v>
+        <v>0.39560439560439559</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="7"/>
-        <v>-1.1190281065829994</v>
+        <v>-8.0547778310761267</v>
       </c>
       <c r="I27" s="1">
         <v>300000</v>
@@ -5226,21 +5244,21 @@
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="D28" s="1">
-        <v>9.2999999999999999E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="E28" s="1">
-        <v>7.9000000000000001E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="6"/>
-        <v>0.84946236559139787</v>
+        <v>0.48351648351648352</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="7"/>
-        <v>-1.4171171452698736</v>
+        <v>-6.3117743166981235</v>
       </c>
       <c r="I28" s="1">
         <v>400000</v>
@@ -5278,6 +5296,23 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D29" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29/D29</f>
+        <v>0.53846153846153855</v>
+      </c>
+      <c r="G29" s="1">
+        <f>20*LOG10(F29)</f>
+        <v>-5.3769062458515968</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -5303,17 +5338,21 @@
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>500000</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="e">
-        <f t="shared" ref="F30" si="10">E30/D30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="1" t="e">
+        <v>300000</v>
+      </c>
+      <c r="D30" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30/D30</f>
+        <v>0.51086956521739135</v>
+      </c>
+      <c r="G30" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-5.8337993881967556</v>
       </c>
       <c r="O30" s="1">
         <v>500000</v>
@@ -5331,6 +5370,25 @@
       <c r="S30" s="1">
         <f t="shared" si="2"/>
         <v>-5.0084000461778793</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>400000</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" ref="F31" si="10">E31/D31</f>
+        <v>0.45652173913043481</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.8107707389530958</v>
       </c>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">

</xml_diff>